<commit_message>
Updated Excel spreadsheet with graphs
</commit_message>
<xml_diff>
--- a/org.topbraid.jmeter.metrics/ComparisonLocksEnabledVsLocksDisabled.xlsx
+++ b/org.topbraid.jmeter.metrics/ComparisonLocksEnabledVsLocksDisabled.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11325" windowHeight="5235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,8 @@
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -698,11 +699,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99181696"/>
-        <c:axId val="99183232"/>
+        <c:axId val="39724544"/>
+        <c:axId val="39726080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99181696"/>
+        <c:axId val="39724544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,7 +712,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99183232"/>
+        <c:crossAx val="39726080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -719,7 +720,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99183232"/>
+        <c:axId val="39726080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -730,7 +731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99181696"/>
+        <c:crossAx val="39724544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1298,11 +1299,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="99205888"/>
-        <c:axId val="99207424"/>
+        <c:axId val="39769216"/>
+        <c:axId val="39770752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="99205888"/>
+        <c:axId val="39769216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,7 +1312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99207424"/>
+        <c:crossAx val="39770752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1319,7 +1320,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99207424"/>
+        <c:axId val="39770752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99205888"/>
+        <c:crossAx val="39769216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2262,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>